<commit_message>
Add new cases for AP6800
Add new cases for AP6800
</commit_message>
<xml_diff>
--- a/NEO_Contact Reader_TW/Contact test case list.xlsx
+++ b/NEO_Contact Reader_TW/Contact test case list.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vivotech\regress\regression\regress_test\test_tree\NEO_Contact Reader_TW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C98B7CF-C9CC-42B0-8971-BB40BFA57259}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B231FDD5-DBB3-48B5-9100-E6375CC7230F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1875" yWindow="1875" windowWidth="13770" windowHeight="12150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5430" yWindow="195" windowWidth="15420" windowHeight="15030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test case list" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="275">
   <si>
     <t>60-10</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4876,6 +4889,25 @@
   <si>
     <t>CR600</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2C-19</t>
+  </si>
+  <si>
+    <t>2C-1A</t>
+  </si>
+  <si>
+    <t>2C-1B</t>
+  </si>
+  <si>
+    <t>2C-1C</t>
+  </si>
+  <si>
+    <t>CR032-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CR032-3</t>
   </si>
 </sst>
 </file>
@@ -5130,14 +5162,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5146,7 +5178,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5155,25 +5187,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5182,13 +5214,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5197,16 +5223,52 @@
     <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5215,232 +5277,7 @@
     <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5455,20 +5292,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5494,9 +5337,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5534,9 +5377,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5569,26 +5412,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5621,26 +5447,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5814,13 +5623,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H156"/>
+  <dimension ref="A1:H160"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B140" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B136" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E157" sqref="E157"/>
+      <selection pane="bottomRight" activeCell="F159" sqref="F159:F160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5837,13 +5646,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="98" t="s">
+      <c r="B1" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="98"/>
+      <c r="C1" s="43"/>
       <c r="D1" s="4" t="s">
         <v>79</v>
       </c>
@@ -5855,19 +5664,19 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="96" t="s">
+      <c r="B2" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E2" s="104" t="s">
+      <c r="D2" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="39" t="s">
         <v>108</v>
       </c>
       <c r="F2" s="9" t="s">
@@ -5876,15 +5685,15 @@
       <c r="H2" s="10"/>
     </row>
     <row r="3" spans="1:8" ht="64.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="101"/>
-      <c r="B3" s="96"/>
-      <c r="C3" s="20" t="s">
+      <c r="A3" s="31"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E3" s="105"/>
+      <c r="D3" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" s="40"/>
       <c r="F3" s="9" t="s">
         <v>95</v>
       </c>
@@ -5893,45 +5702,45 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="101"/>
-      <c r="B4" s="96"/>
-      <c r="C4" s="26" t="s">
+      <c r="A4" s="31"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="E4" s="105"/>
+      <c r="D4" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="40"/>
       <c r="F4" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="101"/>
-      <c r="B5" s="96"/>
-      <c r="C5" s="26" t="s">
+      <c r="A5" s="31"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="D5" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E5" s="106"/>
+      <c r="D5" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" s="41"/>
       <c r="F5" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="33" x14ac:dyDescent="0.25">
-      <c r="A6" s="101"/>
-      <c r="B6" s="20" t="s">
+      <c r="A6" s="31"/>
+      <c r="B6" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="D6" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E6" s="22" t="s">
+      <c r="D6" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>109</v>
       </c>
       <c r="F6" s="9" t="s">
@@ -5939,17 +5748,17 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="101"/>
-      <c r="B7" s="20" t="s">
+      <c r="A7" s="31"/>
+      <c r="B7" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="8" t="s">
         <v>81</v>
       </c>
       <c r="F7" s="17" t="s">
@@ -5957,17 +5766,17 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="144.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="101"/>
-      <c r="B8" s="23" t="s">
+      <c r="A8" s="31"/>
+      <c r="B8" s="20" t="s">
         <v>130</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="D8" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E8" s="22" t="s">
+      <c r="D8" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>165</v>
       </c>
       <c r="F8" s="9" t="s">
@@ -5975,17 +5784,17 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="101"/>
-      <c r="B9" s="25" t="s">
+      <c r="A9" s="31"/>
+      <c r="B9" s="20" t="s">
         <v>191</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="E9" s="32" t="s">
+      <c r="E9" s="8" t="s">
         <v>197</v>
       </c>
       <c r="F9" s="9" t="s">
@@ -5993,17 +5802,17 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="101"/>
-      <c r="B10" s="52" t="s">
+      <c r="A10" s="31"/>
+      <c r="B10" s="20" t="s">
         <v>190</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="8" t="s">
         <v>196</v>
       </c>
       <c r="F10" s="9" t="s">
@@ -6011,14 +5820,14 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="101"/>
-      <c r="B11" s="90" t="s">
+      <c r="A11" s="31"/>
+      <c r="B11" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="11" t="s">
@@ -6029,12 +5838,12 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="101"/>
-      <c r="B12" s="92"/>
-      <c r="C12" s="20" t="s">
+      <c r="A12" s="31"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="11" t="s">
@@ -6045,12 +5854,12 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="101"/>
-      <c r="B13" s="91"/>
-      <c r="C13" s="20" t="s">
+      <c r="A13" s="31"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="11" t="s">
@@ -6061,17 +5870,17 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="101"/>
-      <c r="B14" s="102" t="s">
+      <c r="A14" s="31"/>
+      <c r="B14" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="22" t="s">
+      <c r="E14" s="8" t="s">
         <v>81</v>
       </c>
       <c r="F14" s="17" t="s">
@@ -6079,12 +5888,12 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="33" x14ac:dyDescent="0.25">
-      <c r="A15" s="101"/>
-      <c r="B15" s="103"/>
-      <c r="C15" s="20" t="s">
+      <c r="A15" s="31"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="8" t="s">
         <v>75</v>
       </c>
       <c r="E15" s="11" t="s">
@@ -6095,12 +5904,12 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="66" x14ac:dyDescent="0.25">
-      <c r="A16" s="101"/>
-      <c r="B16" s="103"/>
-      <c r="C16" s="20" t="s">
+      <c r="A16" s="31"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E16" s="8" t="s">
@@ -6111,15 +5920,15 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="66" x14ac:dyDescent="0.25">
-      <c r="A17" s="101"/>
-      <c r="B17" s="103"/>
-      <c r="C17" s="20" t="s">
+      <c r="A17" s="31"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="22" t="s">
+      <c r="E17" s="8" t="s">
         <v>83</v>
       </c>
       <c r="F17" s="17" t="s">
@@ -6127,15 +5936,15 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="66" x14ac:dyDescent="0.25">
-      <c r="A18" s="101"/>
-      <c r="B18" s="103"/>
-      <c r="C18" s="20" t="s">
+      <c r="A18" s="31"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="D18" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E18" s="22" t="s">
+      <c r="D18" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="8" t="s">
         <v>166</v>
       </c>
       <c r="F18" s="9" t="s">
@@ -6143,15 +5952,15 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="66" x14ac:dyDescent="0.25">
-      <c r="A19" s="101"/>
-      <c r="B19" s="103"/>
-      <c r="C19" s="20" t="s">
+      <c r="A19" s="31"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="D19" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E19" s="18" t="s">
+      <c r="D19" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" s="11" t="s">
         <v>232</v>
       </c>
       <c r="F19" s="9" t="s">
@@ -6160,15 +5969,15 @@
       <c r="G19" s="10"/>
     </row>
     <row r="20" spans="1:7" ht="66" x14ac:dyDescent="0.25">
-      <c r="A20" s="101"/>
-      <c r="B20" s="103"/>
-      <c r="C20" s="60" t="s">
+      <c r="A20" s="31"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="D20" s="61" t="s">
+      <c r="D20" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="11" t="s">
         <v>232</v>
       </c>
       <c r="F20" s="17" t="s">
@@ -6177,15 +5986,15 @@
       <c r="G20" s="10"/>
     </row>
     <row r="21" spans="1:7" ht="99" x14ac:dyDescent="0.25">
-      <c r="A21" s="101"/>
-      <c r="B21" s="103"/>
-      <c r="C21" s="20" t="s">
+      <c r="A21" s="31"/>
+      <c r="B21" s="46"/>
+      <c r="C21" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D21" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E21" s="22" t="s">
+      <c r="D21" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" s="8" t="s">
         <v>167</v>
       </c>
       <c r="F21" s="9" t="s">
@@ -6193,15 +6002,15 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A22" s="101"/>
-      <c r="B22" s="103"/>
-      <c r="C22" s="20" t="s">
+      <c r="A22" s="31"/>
+      <c r="B22" s="46"/>
+      <c r="C22" s="18" t="s">
         <v>162</v>
       </c>
-      <c r="D22" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E22" s="22" t="s">
+      <c r="D22" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E22" s="8" t="s">
         <v>168</v>
       </c>
       <c r="F22" s="9" t="s">
@@ -6209,51 +6018,48 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="33" x14ac:dyDescent="0.25">
-      <c r="A23" s="101"/>
-      <c r="B23" s="103"/>
-      <c r="C23" s="20" t="s">
+      <c r="A23" s="31"/>
+      <c r="B23" s="46"/>
+      <c r="C23" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="D23" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E23" s="22"/>
-      <c r="F23" s="19"/>
+      <c r="D23" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" s="8"/>
     </row>
     <row r="24" spans="1:7" ht="33" x14ac:dyDescent="0.25">
-      <c r="A24" s="101"/>
-      <c r="B24" s="103"/>
-      <c r="C24" s="20" t="s">
+      <c r="A24" s="31"/>
+      <c r="B24" s="46"/>
+      <c r="C24" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="D24" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E24" s="22"/>
-      <c r="F24" s="19"/>
+      <c r="D24" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E24" s="8"/>
     </row>
     <row r="25" spans="1:7" ht="33" x14ac:dyDescent="0.25">
-      <c r="A25" s="101"/>
-      <c r="B25" s="103"/>
-      <c r="C25" s="20" t="s">
+      <c r="A25" s="31"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="D25" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E25" s="22"/>
-      <c r="F25" s="19"/>
+      <c r="D25" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:7" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="101"/>
-      <c r="B26" s="103"/>
-      <c r="C26" s="20" t="s">
+      <c r="A26" s="31"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="22" t="s">
+      <c r="D26" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E26" s="22" t="s">
+      <c r="E26" s="8" t="s">
         <v>82</v>
       </c>
       <c r="F26" s="17" t="s">
@@ -6261,15 +6067,15 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="66" x14ac:dyDescent="0.25">
-      <c r="A27" s="101"/>
-      <c r="B27" s="103"/>
-      <c r="C27" s="20" t="s">
+      <c r="A27" s="31"/>
+      <c r="B27" s="46"/>
+      <c r="C27" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="D27" s="22" t="s">
+      <c r="D27" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E27" s="22" t="s">
+      <c r="E27" s="8" t="s">
         <v>82</v>
       </c>
       <c r="F27" s="17" t="s">
@@ -6277,15 +6083,15 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="101"/>
-      <c r="B28" s="103"/>
-      <c r="C28" s="20" t="s">
+      <c r="A28" s="31"/>
+      <c r="B28" s="46"/>
+      <c r="C28" s="18" t="s">
         <v>182</v>
       </c>
-      <c r="D28" s="22" t="s">
+      <c r="D28" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E28" s="22" t="s">
+      <c r="E28" s="8" t="s">
         <v>82</v>
       </c>
       <c r="F28" s="17" t="s">
@@ -6293,15 +6099,15 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A29" s="101"/>
-      <c r="B29" s="103"/>
-      <c r="C29" s="20" t="s">
+      <c r="A29" s="31"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="D29" s="22" t="s">
+      <c r="D29" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E29" s="22" t="s">
+      <c r="E29" s="8" t="s">
         <v>82</v>
       </c>
       <c r="F29" s="17" t="s">
@@ -6309,15 +6115,15 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A30" s="101"/>
-      <c r="B30" s="103"/>
-      <c r="C30" s="20" t="s">
+      <c r="A30" s="31"/>
+      <c r="B30" s="46"/>
+      <c r="C30" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="22" t="s">
+      <c r="D30" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E30" s="22" t="s">
+      <c r="E30" s="8" t="s">
         <v>84</v>
       </c>
       <c r="F30" s="17" t="s">
@@ -6325,15 +6131,15 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A31" s="101"/>
-      <c r="B31" s="103"/>
-      <c r="C31" s="20" t="s">
+      <c r="A31" s="31"/>
+      <c r="B31" s="46"/>
+      <c r="C31" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D31" s="22" t="s">
+      <c r="D31" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="22" t="s">
+      <c r="E31" s="8" t="s">
         <v>85</v>
       </c>
       <c r="F31" s="17" t="s">
@@ -6341,15 +6147,15 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="101"/>
-      <c r="B32" s="103"/>
-      <c r="C32" s="20" t="s">
+      <c r="A32" s="31"/>
+      <c r="B32" s="46"/>
+      <c r="C32" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D32" s="22" t="s">
+      <c r="D32" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="22" t="s">
+      <c r="E32" s="8" t="s">
         <v>85</v>
       </c>
       <c r="F32" s="17" t="s">
@@ -6357,15 +6163,15 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="99" x14ac:dyDescent="0.25">
-      <c r="A33" s="101"/>
-      <c r="B33" s="103"/>
-      <c r="C33" s="20" t="s">
+      <c r="A33" s="31"/>
+      <c r="B33" s="46"/>
+      <c r="C33" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D33" s="22" t="s">
+      <c r="D33" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E33" s="22" t="s">
+      <c r="E33" s="8" t="s">
         <v>85</v>
       </c>
       <c r="F33" s="17" t="s">
@@ -6373,12 +6179,12 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="99" x14ac:dyDescent="0.25">
-      <c r="A34" s="101"/>
-      <c r="B34" s="103"/>
-      <c r="C34" s="20" t="s">
+      <c r="A34" s="31"/>
+      <c r="B34" s="46"/>
+      <c r="C34" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="D34" s="22" t="s">
+      <c r="D34" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E34" s="8" t="s">
@@ -6389,12 +6195,12 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="181.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="101"/>
-      <c r="B35" s="103"/>
-      <c r="C35" s="53" t="s">
+      <c r="A35" s="31"/>
+      <c r="B35" s="46"/>
+      <c r="C35" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="D35" s="22" t="s">
+      <c r="D35" s="8" t="s">
         <v>75</v>
       </c>
       <c r="E35" s="13" t="s">
@@ -6405,15 +6211,15 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="99" x14ac:dyDescent="0.25">
-      <c r="A36" s="101"/>
-      <c r="B36" s="103"/>
-      <c r="C36" s="20" t="s">
+      <c r="A36" s="31"/>
+      <c r="B36" s="46"/>
+      <c r="C36" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="D36" s="22" t="s">
+      <c r="D36" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E36" s="22" t="s">
+      <c r="E36" s="8" t="s">
         <v>83</v>
       </c>
       <c r="F36" s="17" t="s">
@@ -6421,16 +6227,16 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="66" x14ac:dyDescent="0.25">
-      <c r="A37" s="99" t="s">
+      <c r="A37" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="20" t="s">
+      <c r="B37" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C37" s="20" t="s">
+      <c r="C37" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="D37" s="22" t="s">
+      <c r="D37" s="8" t="s">
         <v>75</v>
       </c>
       <c r="E37" s="13" t="s">
@@ -6441,14 +6247,14 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="33" x14ac:dyDescent="0.25">
-      <c r="A38" s="99"/>
-      <c r="B38" s="20" t="s">
+      <c r="A38" s="44"/>
+      <c r="B38" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C38" s="20" t="s">
+      <c r="C38" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="D38" s="22" t="s">
+      <c r="D38" s="8" t="s">
         <v>75</v>
       </c>
       <c r="E38" s="13" t="s">
@@ -6459,17 +6265,17 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="96.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="99"/>
-      <c r="B39" s="23" t="s">
+      <c r="A39" s="44"/>
+      <c r="B39" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="C39" s="20" t="s">
+      <c r="C39" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="D39" s="22" t="s">
+      <c r="D39" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="22" t="s">
+      <c r="E39" s="8" t="s">
         <v>119</v>
       </c>
       <c r="F39" s="17" t="s">
@@ -6477,17 +6283,17 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="99"/>
-      <c r="B40" s="25" t="s">
+      <c r="A40" s="44"/>
+      <c r="B40" s="20" t="s">
         <v>191</v>
       </c>
       <c r="C40" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="D40" s="28" t="s">
+      <c r="D40" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="E40" s="32" t="s">
+      <c r="E40" s="8" t="s">
         <v>197</v>
       </c>
       <c r="F40" s="9" t="s">
@@ -6495,17 +6301,17 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="99"/>
-      <c r="B41" s="90" t="s">
+      <c r="A41" s="44"/>
+      <c r="B41" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="C41" s="20" t="s">
+      <c r="C41" s="18" t="s">
         <v>49</v>
       </c>
       <c r="D41" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="E41" s="22" t="s">
+      <c r="E41" s="8" t="s">
         <v>161</v>
       </c>
       <c r="F41" s="9" t="s">
@@ -6513,15 +6319,15 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="99"/>
-      <c r="B42" s="92"/>
-      <c r="C42" s="20" t="s">
+      <c r="A42" s="44"/>
+      <c r="B42" s="33"/>
+      <c r="C42" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="D42" s="22" t="s">
+      <c r="D42" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E42" s="22" t="s">
+      <c r="E42" s="8" t="s">
         <v>83</v>
       </c>
       <c r="F42" s="17" t="s">
@@ -6529,15 +6335,15 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="66" x14ac:dyDescent="0.25">
-      <c r="A43" s="99"/>
-      <c r="B43" s="91"/>
-      <c r="C43" s="20" t="s">
+      <c r="A43" s="44"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="D43" s="22" t="s">
+      <c r="D43" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E43" s="22" t="s">
+      <c r="E43" s="8" t="s">
         <v>96</v>
       </c>
       <c r="F43" s="17" t="s">
@@ -6545,19 +6351,19 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="66" x14ac:dyDescent="0.25">
-      <c r="A44" s="93" t="s">
+      <c r="A44" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="B44" s="20" t="s">
+      <c r="B44" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C44" s="20" t="s">
+      <c r="C44" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="D44" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E44" s="22" t="s">
+      <c r="D44" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E44" s="8" t="s">
         <v>112</v>
       </c>
       <c r="F44" s="9" t="s">
@@ -6565,17 +6371,17 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="80.25" x14ac:dyDescent="0.25">
-      <c r="A45" s="94"/>
-      <c r="B45" s="23" t="s">
+      <c r="A45" s="48"/>
+      <c r="B45" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="C45" s="20" t="s">
+      <c r="C45" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="D45" s="22" t="s">
+      <c r="D45" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E45" s="22" t="s">
+      <c r="E45" s="8" t="s">
         <v>126</v>
       </c>
       <c r="F45" s="17" t="s">
@@ -6583,17 +6389,17 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="94"/>
-      <c r="B46" s="25" t="s">
+      <c r="A46" s="48"/>
+      <c r="B46" s="20" t="s">
         <v>191</v>
       </c>
       <c r="C46" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="D46" s="28" t="s">
+      <c r="D46" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="E46" s="32" t="s">
+      <c r="E46" s="8" t="s">
         <v>197</v>
       </c>
       <c r="F46" s="9" t="s">
@@ -6601,17 +6407,17 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A47" s="94"/>
-      <c r="B47" s="90" t="s">
+      <c r="A47" s="48"/>
+      <c r="B47" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C47" s="20" t="s">
+      <c r="C47" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="D47" s="22" t="s">
+      <c r="D47" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E47" s="22" t="s">
+      <c r="E47" s="8" t="s">
         <v>83</v>
       </c>
       <c r="F47" s="17" t="s">
@@ -6619,15 +6425,15 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A48" s="95"/>
-      <c r="B48" s="91"/>
-      <c r="C48" s="20" t="s">
+      <c r="A48" s="49"/>
+      <c r="B48" s="29"/>
+      <c r="C48" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="D48" s="22" t="s">
+      <c r="D48" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E48" s="22" t="s">
+      <c r="E48" s="8" t="s">
         <v>85</v>
       </c>
       <c r="F48" s="17" t="s">
@@ -6635,19 +6441,19 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="97" t="s">
+      <c r="A49" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="B49" s="96" t="s">
+      <c r="B49" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="C49" s="20" t="s">
+      <c r="C49" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D49" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E49" s="22" t="s">
+      <c r="D49" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E49" s="8" t="s">
         <v>175</v>
       </c>
       <c r="F49" s="9" t="s">
@@ -6655,15 +6461,15 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="97"/>
-      <c r="B50" s="96"/>
-      <c r="C50" s="20" t="s">
+      <c r="A50" s="37"/>
+      <c r="B50" s="36"/>
+      <c r="C50" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D50" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E50" s="22" t="s">
+      <c r="D50" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E50" s="8" t="s">
         <v>176</v>
       </c>
       <c r="F50" s="9" t="s">
@@ -6671,15 +6477,15 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="97"/>
-      <c r="B51" s="96"/>
-      <c r="C51" s="20" t="s">
+      <c r="A51" s="37"/>
+      <c r="B51" s="36"/>
+      <c r="C51" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D51" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E51" s="22" t="s">
+      <c r="D51" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E51" s="8" t="s">
         <v>177</v>
       </c>
       <c r="F51" s="9" t="s">
@@ -6687,17 +6493,17 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="97"/>
-      <c r="B52" s="62" t="s">
+      <c r="A52" s="37"/>
+      <c r="B52" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="C52" s="20" t="s">
+      <c r="C52" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="D52" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E52" s="22" t="s">
+      <c r="D52" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E52" s="8" t="s">
         <v>178</v>
       </c>
       <c r="F52" s="9" t="s">
@@ -6705,19 +6511,19 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="97" t="s">
+      <c r="A53" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="B53" s="96" t="s">
+      <c r="B53" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="C53" s="20" t="s">
+      <c r="C53" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D53" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E53" s="104" t="s">
+      <c r="D53" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E53" s="39" t="s">
         <v>113</v>
       </c>
       <c r="F53" s="9" t="s">
@@ -6725,31 +6531,31 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="97"/>
-      <c r="B54" s="96"/>
-      <c r="C54" s="20" t="s">
+      <c r="A54" s="37"/>
+      <c r="B54" s="36"/>
+      <c r="C54" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D54" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E54" s="106"/>
+      <c r="D54" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E54" s="41"/>
       <c r="F54" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A55" s="97"/>
-      <c r="B55" s="20" t="s">
+      <c r="A55" s="37"/>
+      <c r="B55" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C55" s="20" t="s">
+      <c r="C55" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D55" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E55" s="22" t="s">
+      <c r="D55" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E55" s="8" t="s">
         <v>114</v>
       </c>
       <c r="F55" s="9" t="s">
@@ -6757,19 +6563,19 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="81.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="97" t="s">
+      <c r="A56" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B56" s="96" t="s">
+      <c r="B56" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="C56" s="20" t="s">
+      <c r="C56" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D56" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E56" s="104" t="s">
+      <c r="D56" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E56" s="39" t="s">
         <v>115</v>
       </c>
       <c r="F56" s="9" t="s">
@@ -6777,31 +6583,31 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="97"/>
-      <c r="B57" s="96"/>
-      <c r="C57" s="20" t="s">
+      <c r="A57" s="37"/>
+      <c r="B57" s="36"/>
+      <c r="C57" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D57" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E57" s="106"/>
+      <c r="D57" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E57" s="41"/>
       <c r="F57" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A58" s="97"/>
-      <c r="B58" s="20" t="s">
+      <c r="A58" s="37"/>
+      <c r="B58" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C58" s="20" t="s">
+      <c r="C58" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D58" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E58" s="104" t="s">
+      <c r="D58" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E58" s="39" t="s">
         <v>114</v>
       </c>
       <c r="F58" s="9" t="s">
@@ -6809,32 +6615,32 @@
       </c>
     </row>
     <row r="59" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A59" s="97"/>
-      <c r="B59" s="20" t="s">
+      <c r="A59" s="37"/>
+      <c r="B59" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="C59" s="20" t="s">
+      <c r="C59" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="D59" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E59" s="106"/>
+      <c r="D59" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E59" s="41"/>
       <c r="F59" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="81.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="97" t="s">
+      <c r="A60" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="B60" s="96" t="s">
+      <c r="B60" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="C60" s="20" t="s">
+      <c r="C60" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="D60" s="22" t="s">
+      <c r="D60" s="8" t="s">
         <v>75</v>
       </c>
       <c r="E60" s="16" t="s">
@@ -6845,12 +6651,12 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="97"/>
-      <c r="B61" s="96"/>
-      <c r="C61" s="20" t="s">
+      <c r="A61" s="37"/>
+      <c r="B61" s="36"/>
+      <c r="C61" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="D61" s="22" t="s">
+      <c r="D61" s="8" t="s">
         <v>75</v>
       </c>
       <c r="E61" s="16" t="s">
@@ -6861,17 +6667,17 @@
       </c>
     </row>
     <row r="62" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A62" s="97"/>
-      <c r="B62" s="20" t="s">
+      <c r="A62" s="37"/>
+      <c r="B62" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C62" s="20" t="s">
+      <c r="C62" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D62" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E62" s="22" t="s">
+      <c r="D62" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E62" s="8" t="s">
         <v>114</v>
       </c>
       <c r="F62" s="9" t="s">
@@ -6879,19 +6685,19 @@
       </c>
     </row>
     <row r="63" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A63" s="97" t="s">
+      <c r="A63" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="B63" s="96" t="s">
+      <c r="B63" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="C63" s="20" t="s">
+      <c r="C63" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D63" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E63" s="104" t="s">
+      <c r="D63" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E63" s="39" t="s">
         <v>133</v>
       </c>
       <c r="F63" s="9" t="s">
@@ -6899,31 +6705,31 @@
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="97"/>
-      <c r="B64" s="96"/>
-      <c r="C64" s="20" t="s">
+      <c r="A64" s="37"/>
+      <c r="B64" s="36"/>
+      <c r="C64" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D64" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E64" s="106"/>
+      <c r="D64" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E64" s="41"/>
       <c r="F64" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="97"/>
-      <c r="B65" s="90" t="s">
+      <c r="A65" s="37"/>
+      <c r="B65" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="C65" s="42" t="s">
+      <c r="C65" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D65" s="43" t="s">
-        <v>75</v>
-      </c>
-      <c r="E65" s="43" t="s">
+      <c r="D65" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E65" s="8" t="s">
         <v>132</v>
       </c>
       <c r="F65" s="9" t="s">
@@ -6931,15 +6737,15 @@
       </c>
     </row>
     <row r="66" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A66" s="97"/>
-      <c r="B66" s="91"/>
-      <c r="C66" s="41" t="s">
+      <c r="A66" s="37"/>
+      <c r="B66" s="29"/>
+      <c r="C66" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="D66" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E66" s="43" t="s">
+      <c r="D66" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E66" s="8" t="s">
         <v>215</v>
       </c>
       <c r="F66" s="9" t="s">
@@ -6947,19 +6753,19 @@
       </c>
     </row>
     <row r="67" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A67" s="97" t="s">
+      <c r="A67" s="37" t="s">
         <v>20</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C67" s="20" t="s">
+      <c r="C67" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D67" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E67" s="79" t="s">
+      <c r="D67" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E67" s="25" t="s">
         <v>134</v>
       </c>
       <c r="F67" s="9" t="s">
@@ -6967,17 +6773,17 @@
       </c>
     </row>
     <row r="68" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="97"/>
+      <c r="A68" s="37"/>
       <c r="B68" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C68" s="20" t="s">
+      <c r="C68" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D68" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E68" s="22" t="s">
+      <c r="D68" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E68" s="8" t="s">
         <v>132</v>
       </c>
       <c r="F68" s="9" t="s">
@@ -6985,19 +6791,19 @@
       </c>
     </row>
     <row r="69" spans="1:6" ht="81.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="97" t="s">
+      <c r="A69" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="B69" s="96" t="s">
+      <c r="B69" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="C69" s="20" t="s">
+      <c r="C69" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="D69" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E69" s="104" t="s">
+      <c r="D69" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E69" s="39" t="s">
         <v>135</v>
       </c>
       <c r="F69" s="9" t="s">
@@ -7005,31 +6811,31 @@
       </c>
     </row>
     <row r="70" spans="1:6" ht="33" x14ac:dyDescent="0.25">
-      <c r="A70" s="97"/>
-      <c r="B70" s="96"/>
-      <c r="C70" s="20" t="s">
+      <c r="A70" s="37"/>
+      <c r="B70" s="36"/>
+      <c r="C70" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="D70" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E70" s="106"/>
+      <c r="D70" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E70" s="41"/>
       <c r="F70" s="12" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A71" s="97"/>
-      <c r="B71" s="20" t="s">
+      <c r="A71" s="37"/>
+      <c r="B71" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C71" s="20" t="s">
+      <c r="C71" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D71" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E71" s="22" t="s">
+      <c r="D71" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E71" s="8" t="s">
         <v>132</v>
       </c>
       <c r="F71" s="9" t="s">
@@ -7037,19 +6843,19 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A72" s="97" t="s">
+      <c r="A72" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="B72" s="96" t="s">
+      <c r="B72" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="C72" s="20" t="s">
+      <c r="C72" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D72" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E72" s="104" t="s">
+      <c r="D72" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E72" s="39" t="s">
         <v>136</v>
       </c>
       <c r="F72" s="9" t="s">
@@ -7057,31 +6863,31 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="97"/>
-      <c r="B73" s="96"/>
-      <c r="C73" s="20" t="s">
+      <c r="A73" s="37"/>
+      <c r="B73" s="36"/>
+      <c r="C73" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="D73" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E73" s="106"/>
+      <c r="D73" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E73" s="41"/>
       <c r="F73" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A74" s="97"/>
-      <c r="B74" s="20" t="s">
+      <c r="A74" s="37"/>
+      <c r="B74" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C74" s="20" t="s">
+      <c r="C74" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D74" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E74" s="22" t="s">
+      <c r="D74" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E74" s="8" t="s">
         <v>114</v>
       </c>
       <c r="F74" s="9" t="s">
@@ -7089,19 +6895,19 @@
       </c>
     </row>
     <row r="75" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A75" s="97" t="s">
+      <c r="A75" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="B75" s="96" t="s">
+      <c r="B75" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="C75" s="20" t="s">
+      <c r="C75" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D75" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E75" s="104" t="s">
+      <c r="D75" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E75" s="39" t="s">
         <v>138</v>
       </c>
       <c r="F75" s="9" t="s">
@@ -7109,45 +6915,45 @@
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="97"/>
-      <c r="B76" s="96"/>
+      <c r="A76" s="37"/>
+      <c r="B76" s="36"/>
       <c r="C76" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D76" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E76" s="105"/>
+      <c r="D76" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E76" s="40"/>
       <c r="F76" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="97"/>
-      <c r="B77" s="96"/>
+      <c r="A77" s="37"/>
+      <c r="B77" s="36"/>
       <c r="C77" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D77" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E77" s="106"/>
+      <c r="D77" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E77" s="41"/>
       <c r="F77" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A78" s="97"/>
-      <c r="B78" s="20" t="s">
+      <c r="A78" s="37"/>
+      <c r="B78" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C78" s="20" t="s">
+      <c r="C78" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D78" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E78" s="22" t="s">
+      <c r="D78" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E78" s="8" t="s">
         <v>137</v>
       </c>
       <c r="F78" s="9" t="s">
@@ -7155,19 +6961,19 @@
       </c>
     </row>
     <row r="79" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A79" s="97" t="s">
+      <c r="A79" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="B79" s="90" t="s">
+      <c r="B79" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="C79" s="20" t="s">
+      <c r="C79" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D79" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E79" s="104" t="s">
+      <c r="D79" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E79" s="39" t="s">
         <v>139</v>
       </c>
       <c r="F79" s="9" t="s">
@@ -7175,45 +6981,45 @@
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="97"/>
-      <c r="B80" s="92"/>
+      <c r="A80" s="37"/>
+      <c r="B80" s="33"/>
       <c r="C80" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D80" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E80" s="105"/>
+      <c r="D80" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E80" s="40"/>
       <c r="F80" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="97"/>
-      <c r="B81" s="91"/>
+      <c r="A81" s="37"/>
+      <c r="B81" s="29"/>
       <c r="C81" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D81" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E81" s="106"/>
+      <c r="D81" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E81" s="41"/>
       <c r="F81" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A82" s="97"/>
-      <c r="B82" s="20" t="s">
+      <c r="A82" s="37"/>
+      <c r="B82" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C82" s="20" t="s">
+      <c r="C82" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D82" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E82" s="104" t="s">
+      <c r="D82" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E82" s="39" t="s">
         <v>137</v>
       </c>
       <c r="F82" s="9" t="s">
@@ -7221,35 +7027,35 @@
       </c>
     </row>
     <row r="83" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A83" s="97"/>
-      <c r="B83" s="20" t="s">
+      <c r="A83" s="37"/>
+      <c r="B83" s="18" t="s">
         <v>27</v>
       </c>
       <c r="C83" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D83" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E83" s="106"/>
+      <c r="D83" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E83" s="41"/>
       <c r="F83" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A84" s="97" t="s">
+      <c r="A84" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="B84" s="96" t="s">
+      <c r="B84" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="C84" s="20" t="s">
+      <c r="C84" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D84" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E84" s="104" t="s">
+      <c r="D84" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E84" s="39" t="s">
         <v>140</v>
       </c>
       <c r="F84" s="9" t="s">
@@ -7257,45 +7063,45 @@
       </c>
     </row>
     <row r="85" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A85" s="97"/>
-      <c r="B85" s="96"/>
-      <c r="C85" s="20" t="s">
+      <c r="A85" s="37"/>
+      <c r="B85" s="36"/>
+      <c r="C85" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="D85" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E85" s="105"/>
+      <c r="D85" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E85" s="40"/>
       <c r="F85" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="97"/>
-      <c r="B86" s="96"/>
+      <c r="A86" s="37"/>
+      <c r="B86" s="36"/>
       <c r="C86" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D86" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E86" s="106"/>
+      <c r="D86" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E86" s="41"/>
       <c r="F86" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A87" s="97"/>
-      <c r="B87" s="20" t="s">
+      <c r="A87" s="37"/>
+      <c r="B87" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C87" s="20" t="s">
+      <c r="C87" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D87" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E87" s="22" t="s">
+      <c r="D87" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E87" s="8" t="s">
         <v>137</v>
       </c>
       <c r="F87" s="9" t="s">
@@ -7303,19 +7109,19 @@
       </c>
     </row>
     <row r="88" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A88" s="97" t="s">
+      <c r="A88" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="B88" s="96" t="s">
+      <c r="B88" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="C88" s="20" t="s">
+      <c r="C88" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D88" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E88" s="104" t="s">
+      <c r="D88" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E88" s="39" t="s">
         <v>142</v>
       </c>
       <c r="F88" s="9" t="s">
@@ -7323,31 +7129,31 @@
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="97"/>
-      <c r="B89" s="96"/>
+      <c r="A89" s="37"/>
+      <c r="B89" s="36"/>
       <c r="C89" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D89" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E89" s="106"/>
+      <c r="D89" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E89" s="41"/>
       <c r="F89" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A90" s="97"/>
-      <c r="B90" s="20" t="s">
+      <c r="A90" s="37"/>
+      <c r="B90" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C90" s="20" t="s">
+      <c r="C90" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D90" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E90" s="22" t="s">
+      <c r="D90" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E90" s="8" t="s">
         <v>137</v>
       </c>
       <c r="F90" s="9" t="s">
@@ -7355,19 +7161,19 @@
       </c>
     </row>
     <row r="91" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A91" s="97" t="s">
+      <c r="A91" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="B91" s="96" t="s">
+      <c r="B91" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="C91" s="20" t="s">
+      <c r="C91" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D91" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E91" s="104" t="s">
+      <c r="D91" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E91" s="39" t="s">
         <v>143</v>
       </c>
       <c r="F91" s="9" t="s">
@@ -7375,31 +7181,31 @@
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="97"/>
-      <c r="B92" s="96"/>
+      <c r="A92" s="37"/>
+      <c r="B92" s="36"/>
       <c r="C92" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D92" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E92" s="106"/>
+      <c r="D92" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E92" s="41"/>
       <c r="F92" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A93" s="97"/>
-      <c r="B93" s="20" t="s">
+      <c r="A93" s="37"/>
+      <c r="B93" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C93" s="20" t="s">
+      <c r="C93" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D93" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E93" s="22" t="s">
+      <c r="D93" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E93" s="8" t="s">
         <v>141</v>
       </c>
       <c r="F93" s="9" t="s">
@@ -7407,19 +7213,19 @@
       </c>
     </row>
     <row r="94" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A94" s="97" t="s">
+      <c r="A94" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="B94" s="20" t="s">
+      <c r="B94" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="C94" s="20" t="s">
+      <c r="C94" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D94" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E94" s="79" t="s">
+      <c r="D94" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E94" s="25" t="s">
         <v>144</v>
       </c>
       <c r="F94" s="9" t="s">
@@ -7427,17 +7233,17 @@
       </c>
     </row>
     <row r="95" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A95" s="97"/>
-      <c r="B95" s="20" t="s">
+      <c r="A95" s="37"/>
+      <c r="B95" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="C95" s="20" t="s">
+      <c r="C95" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D95" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E95" s="104" t="s">
+      <c r="D95" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E95" s="39" t="s">
         <v>141</v>
       </c>
       <c r="F95" s="9" t="s">
@@ -7445,35 +7251,35 @@
       </c>
     </row>
     <row r="96" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A96" s="97"/>
-      <c r="B96" s="20" t="s">
+      <c r="A96" s="37"/>
+      <c r="B96" s="18" t="s">
         <v>67</v>
       </c>
       <c r="C96" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="D96" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E96" s="106"/>
+      <c r="D96" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E96" s="41"/>
       <c r="F96" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A97" s="97" t="s">
+      <c r="A97" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="B97" s="96" t="s">
+      <c r="B97" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="C97" s="20" t="s">
+      <c r="C97" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D97" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E97" s="80" t="s">
+      <c r="D97" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E97" s="26" t="s">
         <v>145</v>
       </c>
       <c r="F97" s="9" t="s">
@@ -7482,12 +7288,12 @@
       <c r="H97" s="10"/>
     </row>
     <row r="98" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A98" s="97"/>
-      <c r="B98" s="96"/>
-      <c r="C98" s="22" t="s">
+      <c r="A98" s="37"/>
+      <c r="B98" s="36"/>
+      <c r="C98" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D98" s="22" t="s">
+      <c r="D98" s="8" t="s">
         <v>75</v>
       </c>
       <c r="E98" s="13" t="s">
@@ -7498,17 +7304,17 @@
       </c>
     </row>
     <row r="99" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A99" s="97"/>
-      <c r="B99" s="20" t="s">
+      <c r="A99" s="37"/>
+      <c r="B99" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C99" s="20" t="s">
+      <c r="C99" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D99" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E99" s="22" t="s">
+      <c r="D99" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E99" s="8" t="s">
         <v>141</v>
       </c>
       <c r="F99" s="9" t="s">
@@ -7516,60 +7322,60 @@
       </c>
     </row>
     <row r="100" spans="1:8" ht="66" x14ac:dyDescent="0.25">
-      <c r="A100" s="97" t="s">
+      <c r="A100" s="37" t="s">
         <v>37</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C100" s="20" t="s">
+      <c r="C100" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D100" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E100" s="104" t="s">
+      <c r="D100" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E100" s="39" t="s">
         <v>147</v>
       </c>
       <c r="F100" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="G100" s="24" t="s">
+      <c r="G100" s="21" t="s">
         <v>183</v>
       </c>
       <c r="H100" s="10"/>
     </row>
     <row r="101" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A101" s="97"/>
+      <c r="A101" s="37"/>
       <c r="B101" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C101" s="20" t="s">
+      <c r="C101" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D101" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E101" s="106"/>
+      <c r="D101" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E101" s="41"/>
       <c r="F101" s="14" t="s">
         <v>95</v>
       </c>
       <c r="G101" s="10"/>
     </row>
     <row r="102" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A102" s="97" t="s">
+      <c r="A102" s="37" t="s">
         <v>38</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C102" s="20" t="s">
+      <c r="C102" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D102" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E102" s="104" t="s">
+      <c r="D102" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E102" s="39" t="s">
         <v>148</v>
       </c>
       <c r="F102" s="9" t="s">
@@ -7577,35 +7383,35 @@
       </c>
     </row>
     <row r="103" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A103" s="97"/>
+      <c r="A103" s="37"/>
       <c r="B103" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C103" s="20" t="s">
+      <c r="C103" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D103" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E103" s="106"/>
+      <c r="D103" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E103" s="41"/>
       <c r="F103" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A104" s="97" t="s">
+      <c r="A104" s="37" t="s">
         <v>39</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C104" s="20" t="s">
+      <c r="C104" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D104" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E104" s="104" t="s">
+      <c r="D104" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E104" s="39" t="s">
         <v>149</v>
       </c>
       <c r="F104" s="9" t="s">
@@ -7613,35 +7419,35 @@
       </c>
     </row>
     <row r="105" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A105" s="97"/>
+      <c r="A105" s="37"/>
       <c r="B105" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C105" s="20" t="s">
+      <c r="C105" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D105" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E105" s="106"/>
+      <c r="D105" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E105" s="41"/>
       <c r="F105" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A106" s="97" t="s">
+      <c r="A106" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="B106" s="20" t="s">
+      <c r="B106" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="C106" s="20" t="s">
+      <c r="C106" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D106" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E106" s="104" t="s">
+      <c r="D106" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E106" s="39" t="s">
         <v>150</v>
       </c>
       <c r="F106" s="9" t="s">
@@ -7649,35 +7455,35 @@
       </c>
     </row>
     <row r="107" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A107" s="97"/>
-      <c r="B107" s="20" t="s">
+      <c r="A107" s="37"/>
+      <c r="B107" s="18" t="s">
         <v>53</v>
       </c>
       <c r="C107" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D107" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E107" s="106"/>
+      <c r="D107" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E107" s="41"/>
       <c r="F107" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="108" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A108" s="97" t="s">
+      <c r="A108" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="B108" s="20" t="s">
+      <c r="B108" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="C108" s="20" t="s">
+      <c r="C108" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D108" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E108" s="104" t="s">
+      <c r="D108" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E108" s="39" t="s">
         <v>151</v>
       </c>
       <c r="F108" s="9" t="s">
@@ -7685,35 +7491,35 @@
       </c>
     </row>
     <row r="109" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A109" s="97"/>
-      <c r="B109" s="20" t="s">
+      <c r="A109" s="37"/>
+      <c r="B109" s="18" t="s">
         <v>53</v>
       </c>
       <c r="C109" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D109" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E109" s="106"/>
+      <c r="D109" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E109" s="41"/>
       <c r="F109" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="110" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A110" s="97" t="s">
+      <c r="A110" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="B110" s="20" t="s">
+      <c r="B110" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="C110" s="20" t="s">
+      <c r="C110" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D110" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E110" s="79" t="s">
+      <c r="D110" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E110" s="25" t="s">
         <v>157</v>
       </c>
       <c r="F110" s="9" t="s">
@@ -7721,17 +7527,17 @@
       </c>
     </row>
     <row r="111" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A111" s="97"/>
-      <c r="B111" s="96" t="s">
+      <c r="A111" s="37"/>
+      <c r="B111" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="C111" s="20" t="s">
+      <c r="C111" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="D111" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E111" s="104" t="s">
+      <c r="D111" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E111" s="39" t="s">
         <v>152</v>
       </c>
       <c r="F111" s="9" t="s">
@@ -7739,47 +7545,47 @@
       </c>
     </row>
     <row r="112" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A112" s="97"/>
-      <c r="B112" s="96"/>
-      <c r="C112" s="20" t="s">
+      <c r="A112" s="37"/>
+      <c r="B112" s="36"/>
+      <c r="C112" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="D112" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E112" s="105"/>
+      <c r="D112" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E112" s="40"/>
       <c r="F112" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="113" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A113" s="97"/>
-      <c r="B113" s="96"/>
-      <c r="C113" s="20" t="s">
+      <c r="A113" s="37"/>
+      <c r="B113" s="36"/>
+      <c r="C113" s="18" t="s">
         <v>153</v>
       </c>
-      <c r="D113" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E113" s="105"/>
+      <c r="D113" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E113" s="40"/>
       <c r="F113" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="114" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A114" s="97" t="s">
+      <c r="A114" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="B114" s="20" t="s">
+      <c r="B114" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="C114" s="20" t="s">
+      <c r="C114" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D114" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E114" s="22" t="s">
+      <c r="D114" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E114" s="8" t="s">
         <v>158</v>
       </c>
       <c r="F114" s="9" t="s">
@@ -7787,17 +7593,17 @@
       </c>
     </row>
     <row r="115" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A115" s="97"/>
-      <c r="B115" s="20" t="s">
+      <c r="A115" s="37"/>
+      <c r="B115" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="C115" s="20" t="s">
+      <c r="C115" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D115" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E115" s="104" t="s">
+      <c r="D115" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E115" s="39" t="s">
         <v>156</v>
       </c>
       <c r="F115" s="12" t="s">
@@ -7805,63 +7611,63 @@
       </c>
     </row>
     <row r="116" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A116" s="97"/>
-      <c r="B116" s="20" t="s">
+      <c r="A116" s="37"/>
+      <c r="B116" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="C116" s="20" t="s">
+      <c r="C116" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D116" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E116" s="105"/>
+      <c r="D116" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E116" s="40"/>
       <c r="F116" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="97"/>
-      <c r="B117" s="20" t="s">
+      <c r="A117" s="37"/>
+      <c r="B117" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="C117" s="96" t="s">
+      <c r="C117" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="D117" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E117" s="105"/>
-      <c r="F117" s="108" t="s">
+      <c r="D117" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E117" s="40"/>
+      <c r="F117" s="38" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="118" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="97"/>
-      <c r="B118" s="20" t="s">
+      <c r="A118" s="37"/>
+      <c r="B118" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="C118" s="96"/>
-      <c r="D118" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E118" s="106"/>
-      <c r="F118" s="108"/>
+      <c r="C118" s="36"/>
+      <c r="D118" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E118" s="41"/>
+      <c r="F118" s="38"/>
     </row>
     <row r="119" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A119" s="97" t="s">
+      <c r="A119" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="B119" s="20" t="s">
+      <c r="B119" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="C119" s="20" t="s">
+      <c r="C119" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D119" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E119" s="22" t="s">
+      <c r="D119" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E119" s="8" t="s">
         <v>158</v>
       </c>
       <c r="F119" s="9" t="s">
@@ -7869,17 +7675,17 @@
       </c>
     </row>
     <row r="120" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A120" s="97"/>
-      <c r="B120" s="20" t="s">
+      <c r="A120" s="37"/>
+      <c r="B120" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="C120" s="20" t="s">
+      <c r="C120" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D120" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E120" s="105" t="s">
+      <c r="D120" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E120" s="40" t="s">
         <v>159</v>
       </c>
       <c r="F120" s="9" t="s">
@@ -7887,51 +7693,51 @@
       </c>
     </row>
     <row r="121" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A121" s="97"/>
-      <c r="B121" s="20" t="s">
+      <c r="A121" s="37"/>
+      <c r="B121" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="C121" s="20" t="s">
+      <c r="C121" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="D121" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E121" s="105"/>
+      <c r="D121" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E121" s="40"/>
       <c r="F121" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="122" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A122" s="97"/>
-      <c r="B122" s="20" t="s">
+      <c r="A122" s="37"/>
+      <c r="B122" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="C122" s="20" t="s">
+      <c r="C122" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="D122" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E122" s="106"/>
+      <c r="D122" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E122" s="41"/>
       <c r="F122" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A123" s="97" t="s">
+      <c r="A123" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="B123" s="20" t="s">
+      <c r="B123" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="C123" s="20" t="s">
+      <c r="C123" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D123" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E123" s="22" t="s">
+      <c r="D123" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E123" s="8" t="s">
         <v>158</v>
       </c>
       <c r="F123" s="9" t="s">
@@ -7939,17 +7745,17 @@
       </c>
     </row>
     <row r="124" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A124" s="97"/>
-      <c r="B124" s="20" t="s">
+      <c r="A124" s="37"/>
+      <c r="B124" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="C124" s="20" t="s">
+      <c r="C124" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D124" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E124" s="107" t="s">
+      <c r="D124" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E124" s="42" t="s">
         <v>160</v>
       </c>
       <c r="F124" s="9" t="s">
@@ -7957,49 +7763,49 @@
       </c>
     </row>
     <row r="125" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A125" s="97"/>
-      <c r="B125" s="20" t="s">
+      <c r="A125" s="37"/>
+      <c r="B125" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="C125" s="20" t="s">
+      <c r="C125" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="D125" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E125" s="107"/>
+      <c r="D125" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E125" s="42"/>
       <c r="F125" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="126" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A126" s="97"/>
-      <c r="B126" s="20" t="s">
+      <c r="A126" s="37"/>
+      <c r="B126" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="C126" s="20" t="s">
+      <c r="C126" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="D126" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E126" s="107"/>
+      <c r="D126" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E126" s="42"/>
       <c r="F126" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="127" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A127" s="27"/>
-      <c r="B127" s="29" t="s">
+      <c r="A127" s="19"/>
+      <c r="B127" s="18" t="s">
         <v>195</v>
       </c>
-      <c r="C127" s="26" t="s">
+      <c r="C127" s="18" t="s">
         <v>193</v>
       </c>
-      <c r="D127" s="28" t="s">
+      <c r="D127" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="E127" s="30" t="s">
+      <c r="E127" s="8" t="s">
         <v>194</v>
       </c>
       <c r="F127" s="9" t="s">
@@ -8007,50 +7813,50 @@
       </c>
     </row>
     <row r="128" spans="1:6" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="34"/>
-      <c r="B128" s="33"/>
-      <c r="C128" s="33" t="s">
+      <c r="A128" s="19"/>
+      <c r="B128" s="18"/>
+      <c r="C128" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="D128" s="38" t="s">
+      <c r="D128" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="E128" s="35" t="s">
+      <c r="E128" s="8" t="s">
         <v>199</v>
       </c>
       <c r="F128" s="9" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A129" s="100" t="s">
+    <row r="129" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A129" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B129" s="36" t="s">
+      <c r="B129" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="C129" s="36" t="s">
+      <c r="C129" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D129" s="38" t="s">
+      <c r="D129" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="E129" s="40" t="s">
+      <c r="E129" s="8" t="s">
         <v>212</v>
       </c>
       <c r="F129" s="9" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="101"/>
-      <c r="B130" s="110" t="s">
+    <row r="130" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="31"/>
+      <c r="B130" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="C130" s="39" t="s">
+      <c r="C130" s="18" t="s">
         <v>211</v>
       </c>
-      <c r="D130" s="38" t="s">
+      <c r="D130" s="8" t="s">
         <v>189</v>
       </c>
       <c r="E130" s="16" t="s">
@@ -8060,13 +7866,13 @@
         <v>95</v>
       </c>
     </row>
-    <row r="131" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="109"/>
-      <c r="B131" s="111"/>
-      <c r="C131" s="36" t="s">
+    <row r="131" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="32"/>
+      <c r="B131" s="35"/>
+      <c r="C131" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D131" s="38" t="s">
+      <c r="D131" s="8" t="s">
         <v>189</v>
       </c>
       <c r="E131" s="16" t="s">
@@ -8076,234 +7882,233 @@
         <v>95</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A132" s="112" t="s">
+    <row r="132" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A132" s="27" t="s">
         <v>201</v>
       </c>
-      <c r="B132" s="36" t="s">
+      <c r="B132" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="C132" s="36" t="s">
+      <c r="C132" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D132" s="38" t="s">
+      <c r="D132" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="E132" s="79" t="s">
+      <c r="E132" s="25" t="s">
         <v>209</v>
       </c>
       <c r="F132" s="9" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="63" x14ac:dyDescent="0.25">
-      <c r="A133" s="112"/>
-      <c r="B133" s="44" t="s">
+    <row r="133" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+      <c r="A133" s="27"/>
+      <c r="B133" s="23" t="s">
         <v>203</v>
       </c>
-      <c r="C133" s="42" t="s">
+      <c r="C133" s="18" t="s">
         <v>213</v>
       </c>
-      <c r="D133" s="38" t="s">
+      <c r="D133" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="E133" s="40" t="s">
+      <c r="E133" s="8" t="s">
         <v>208</v>
       </c>
       <c r="F133" s="9" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="80.25" x14ac:dyDescent="0.25">
-      <c r="A134" s="45" t="s">
+    <row r="134" spans="1:6" ht="80.25" x14ac:dyDescent="0.25">
+      <c r="A134" s="24" t="s">
         <v>204</v>
       </c>
-      <c r="B134" s="41"/>
-      <c r="C134" s="46" t="s">
+      <c r="B134" s="22"/>
+      <c r="C134" s="18" t="s">
         <v>216</v>
       </c>
-      <c r="D134" s="38" t="s">
+      <c r="D134" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="E134" s="40" t="s">
+      <c r="E134" s="8" t="s">
         <v>210</v>
       </c>
       <c r="F134" s="9" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="79.5" x14ac:dyDescent="0.25">
-      <c r="A135" s="37"/>
-      <c r="B135" s="36" t="s">
+    <row r="135" spans="1:6" ht="79.5" x14ac:dyDescent="0.25">
+      <c r="A135" s="19"/>
+      <c r="B135" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="C135" s="36" t="s">
+      <c r="C135" s="18" t="s">
         <v>205</v>
       </c>
-      <c r="D135" s="38" t="s">
+      <c r="D135" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="E135" s="40" t="s">
+      <c r="E135" s="8" t="s">
         <v>206</v>
       </c>
       <c r="F135" s="9" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="82.5" x14ac:dyDescent="0.25">
-      <c r="A136" s="49" t="s">
+    <row r="136" spans="1:6" ht="82.5" x14ac:dyDescent="0.25">
+      <c r="A136" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="B136" s="48" t="s">
+      <c r="B136" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="C136" s="51" t="s">
+      <c r="C136" s="18" t="s">
         <v>221</v>
       </c>
-      <c r="D136" s="47" t="s">
+      <c r="D136" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="E136" s="50" t="s">
+      <c r="E136" s="8" t="s">
         <v>218</v>
       </c>
       <c r="F136" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="H136" s="19"/>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A137" s="55"/>
-      <c r="B137" s="54" t="s">
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137" s="19"/>
+      <c r="B137" s="18" t="s">
         <v>226</v>
       </c>
-      <c r="C137" s="54" t="s">
+      <c r="C137" s="18" t="s">
         <v>224</v>
       </c>
-      <c r="D137" s="56" t="s">
-        <v>75</v>
-      </c>
-      <c r="E137" s="56" t="s">
+      <c r="D137" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E137" s="8" t="s">
         <v>223</v>
       </c>
       <c r="F137" s="9" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="138" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A138" s="55"/>
-      <c r="B138" s="54" t="s">
+    <row r="138" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A138" s="19"/>
+      <c r="B138" s="18" t="s">
         <v>226</v>
       </c>
-      <c r="C138" s="54" t="s">
+      <c r="C138" s="18" t="s">
         <v>227</v>
       </c>
-      <c r="D138" s="56" t="s">
-        <v>75</v>
-      </c>
-      <c r="E138" s="56" t="s">
+      <c r="D138" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E138" s="8" t="s">
         <v>225</v>
       </c>
       <c r="F138" s="9" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="139" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A139" s="58"/>
-      <c r="B139" s="57" t="s">
+    <row r="139" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A139" s="19"/>
+      <c r="B139" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="C139" s="57" t="s">
+      <c r="C139" s="18" t="s">
         <v>230</v>
       </c>
-      <c r="D139" s="65" t="s">
-        <v>75</v>
-      </c>
-      <c r="E139" s="59" t="s">
+      <c r="D139" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E139" s="8" t="s">
         <v>229</v>
       </c>
       <c r="F139" s="9" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A140" s="64" t="s">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140" s="19" t="s">
         <v>234</v>
       </c>
-      <c r="B140" s="63"/>
-      <c r="C140" s="63" t="s">
+      <c r="B140" s="18"/>
+      <c r="C140" s="18" t="s">
         <v>236</v>
       </c>
-      <c r="D140" s="68" t="s">
-        <v>75</v>
-      </c>
-      <c r="E140" s="65" t="s">
+      <c r="D140" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E140" s="8" t="s">
         <v>235</v>
       </c>
       <c r="F140" s="9" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="141" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A141" s="67" t="s">
+    <row r="141" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A141" s="19" t="s">
         <v>237</v>
       </c>
-      <c r="B141" s="66"/>
-      <c r="C141" s="66" t="s">
+      <c r="B141" s="18"/>
+      <c r="C141" s="18" t="s">
         <v>238</v>
       </c>
-      <c r="D141" s="68" t="s">
-        <v>75</v>
-      </c>
-      <c r="E141" s="68" t="s">
+      <c r="D141" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E141" s="8" t="s">
         <v>239</v>
       </c>
       <c r="F141" s="9" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="142" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="70"/>
-      <c r="B142" s="69" t="s">
+    <row r="142" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="19"/>
+      <c r="B142" s="18" t="s">
         <v>240</v>
       </c>
-      <c r="C142" s="53" t="s">
+      <c r="C142" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="D142" s="71" t="s">
-        <v>75</v>
-      </c>
-      <c r="E142" s="71"/>
-    </row>
-    <row r="143" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="100" t="s">
+      <c r="D142" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E142" s="8"/>
+    </row>
+    <row r="143" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="B143" s="90" t="s">
+      <c r="B143" s="28" t="s">
         <v>248</v>
       </c>
-      <c r="C143" s="72" t="s">
+      <c r="C143" s="18" t="s">
         <v>249</v>
       </c>
-      <c r="D143" s="73" t="s">
+      <c r="D143" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="E143" s="73" t="s">
+      <c r="E143" s="8" t="s">
         <v>244</v>
       </c>
       <c r="F143" s="9" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A144" s="101"/>
-      <c r="B144" s="92"/>
-      <c r="C144" s="72" t="s">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144" s="31"/>
+      <c r="B144" s="33"/>
+      <c r="C144" s="18" t="s">
         <v>250</v>
       </c>
-      <c r="D144" s="73" t="s">
+      <c r="D144" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="E144" s="73" t="s">
+      <c r="E144" s="8" t="s">
         <v>245</v>
       </c>
       <c r="F144" s="9" t="s">
@@ -8311,15 +8116,15 @@
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A145" s="101"/>
-      <c r="B145" s="92"/>
-      <c r="C145" s="72" t="s">
+      <c r="A145" s="31"/>
+      <c r="B145" s="33"/>
+      <c r="C145" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="D145" s="73" t="s">
+      <c r="D145" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="E145" s="73" t="s">
+      <c r="E145" s="8" t="s">
         <v>246</v>
       </c>
       <c r="F145" s="9" t="s">
@@ -8327,15 +8132,15 @@
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A146" s="109"/>
-      <c r="B146" s="91"/>
-      <c r="C146" s="72" t="s">
+      <c r="A146" s="32"/>
+      <c r="B146" s="29"/>
+      <c r="C146" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="D146" s="73" t="s">
+      <c r="D146" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="E146" s="73" t="s">
+      <c r="E146" s="8" t="s">
         <v>247</v>
       </c>
       <c r="F146" s="9" t="s">
@@ -8343,19 +8148,19 @@
       </c>
     </row>
     <row r="147" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="112" t="s">
+      <c r="A147" s="27" t="s">
         <v>253</v>
       </c>
-      <c r="B147" s="90" t="s">
+      <c r="B147" s="28" t="s">
         <v>256</v>
       </c>
-      <c r="C147" s="74" t="s">
+      <c r="C147" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="D147" s="75" t="s">
-        <v>75</v>
-      </c>
-      <c r="E147" s="75" t="s">
+      <c r="D147" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E147" s="8" t="s">
         <v>258</v>
       </c>
       <c r="F147" s="9" t="s">
@@ -8363,15 +8168,15 @@
       </c>
     </row>
     <row r="148" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="112"/>
-      <c r="B148" s="91"/>
-      <c r="C148" s="74" t="s">
+      <c r="A148" s="27"/>
+      <c r="B148" s="29"/>
+      <c r="C148" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="D148" s="75" t="s">
-        <v>75</v>
-      </c>
-      <c r="E148" s="75" t="s">
+      <c r="D148" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E148" s="8" t="s">
         <v>259</v>
       </c>
       <c r="F148" s="9" t="s">
@@ -8379,19 +8184,19 @@
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A149" s="112" t="s">
+      <c r="A149" s="27" t="s">
         <v>253</v>
       </c>
-      <c r="B149" s="90" t="s">
+      <c r="B149" s="28" t="s">
         <v>255</v>
       </c>
-      <c r="C149" s="74" t="s">
+      <c r="C149" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="D149" s="75" t="s">
-        <v>75</v>
-      </c>
-      <c r="E149" s="75" t="s">
+      <c r="D149" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E149" s="8" t="s">
         <v>258</v>
       </c>
       <c r="F149" s="9" t="s">
@@ -8399,15 +8204,15 @@
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A150" s="112"/>
-      <c r="B150" s="91"/>
-      <c r="C150" s="74" t="s">
+      <c r="A150" s="27"/>
+      <c r="B150" s="29"/>
+      <c r="C150" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="D150" s="75" t="s">
-        <v>75</v>
-      </c>
-      <c r="E150" s="75" t="s">
+      <c r="D150" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E150" s="8" t="s">
         <v>259</v>
       </c>
       <c r="F150" s="9" t="s">
@@ -8415,47 +8220,47 @@
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A151" s="112" t="s">
+      <c r="A151" s="27" t="s">
         <v>253</v>
       </c>
-      <c r="B151" s="90" t="s">
+      <c r="B151" s="28" t="s">
         <v>257</v>
       </c>
-      <c r="C151" s="74" t="s">
+      <c r="C151" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="D151" s="75" t="s">
-        <v>75</v>
-      </c>
-      <c r="E151" s="75" t="s">
+      <c r="D151" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E151" s="8" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A152" s="112"/>
-      <c r="B152" s="91"/>
-      <c r="C152" s="74" t="s">
+      <c r="A152" s="27"/>
+      <c r="B152" s="29"/>
+      <c r="C152" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="D152" s="75" t="s">
-        <v>75</v>
-      </c>
-      <c r="E152" s="75" t="s">
+      <c r="D152" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E152" s="8" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A153" s="82"/>
-      <c r="B153" s="81" t="s">
+      <c r="A153" s="19"/>
+      <c r="B153" s="18" t="s">
         <v>226</v>
       </c>
-      <c r="C153" s="81" t="s">
+      <c r="C153" s="18" t="s">
         <v>264</v>
       </c>
-      <c r="D153" s="83" t="s">
-        <v>75</v>
-      </c>
-      <c r="E153" s="83" t="s">
+      <c r="D153" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E153" s="8" t="s">
         <v>263</v>
       </c>
       <c r="F153" s="9" t="s">
@@ -8463,17 +8268,17 @@
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A154" s="77"/>
-      <c r="B154" s="76" t="s">
+      <c r="A154" s="19"/>
+      <c r="B154" s="18" t="s">
         <v>260</v>
       </c>
-      <c r="C154" s="76" t="s">
+      <c r="C154" s="18" t="s">
         <v>261</v>
       </c>
-      <c r="D154" s="78" t="s">
-        <v>75</v>
-      </c>
-      <c r="E154" s="83" t="s">
+      <c r="D154" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E154" s="8" t="s">
         <v>262</v>
       </c>
       <c r="F154" s="9" t="s">
@@ -8481,15 +8286,15 @@
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A155" s="85"/>
-      <c r="B155" s="84" t="s">
+      <c r="A155" s="19"/>
+      <c r="B155" s="18" t="s">
         <v>265</v>
       </c>
-      <c r="C155" s="84"/>
-      <c r="D155" s="86" t="s">
-        <v>75</v>
-      </c>
-      <c r="E155" s="86" t="s">
+      <c r="C155" s="18"/>
+      <c r="D155" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E155" s="8" t="s">
         <v>266</v>
       </c>
       <c r="F155" s="9" t="s">
@@ -8497,73 +8302,97 @@
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A156" s="88"/>
-      <c r="B156" s="87" t="s">
+      <c r="A156" s="19"/>
+      <c r="B156" s="18" t="s">
         <v>267</v>
       </c>
-      <c r="C156" s="87"/>
-      <c r="D156" s="89" t="s">
-        <v>75</v>
-      </c>
-      <c r="E156" s="89" t="s">
+      <c r="C156" s="18"/>
+      <c r="D156" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E156" s="8" t="s">
         <v>268</v>
       </c>
       <c r="F156" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A157" s="19" t="s">
+        <v>269</v>
+      </c>
+      <c r="B157" s="18"/>
+      <c r="C157" s="18"/>
+      <c r="D157" s="8"/>
+      <c r="E157" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="F157" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A158" s="19" t="s">
+        <v>270</v>
+      </c>
+      <c r="B158" s="18"/>
+      <c r="C158" s="18"/>
+      <c r="D158" s="8"/>
+      <c r="E158" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="F158" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A159" s="19" t="s">
+        <v>271</v>
+      </c>
+      <c r="B159" s="18"/>
+      <c r="C159" s="18"/>
+      <c r="D159" s="8"/>
+      <c r="E159" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="F159" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A160" s="19" t="s">
+        <v>272</v>
+      </c>
+      <c r="B160" s="18"/>
+      <c r="C160" s="18"/>
+      <c r="D160" s="8"/>
+      <c r="E160" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="F160" s="9" t="s">
         <v>95</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="84">
-    <mergeCell ref="A147:A148"/>
-    <mergeCell ref="B147:B148"/>
-    <mergeCell ref="A149:A150"/>
-    <mergeCell ref="B149:B150"/>
-    <mergeCell ref="A151:A152"/>
-    <mergeCell ref="B151:B152"/>
-    <mergeCell ref="A143:A146"/>
-    <mergeCell ref="B143:B146"/>
-    <mergeCell ref="A129:A131"/>
-    <mergeCell ref="B130:B131"/>
-    <mergeCell ref="C117:C118"/>
-    <mergeCell ref="A114:A118"/>
-    <mergeCell ref="A132:A133"/>
-    <mergeCell ref="F117:F118"/>
-    <mergeCell ref="E115:E118"/>
-    <mergeCell ref="E84:E86"/>
-    <mergeCell ref="E88:E89"/>
-    <mergeCell ref="E91:E92"/>
-    <mergeCell ref="E95:E96"/>
-    <mergeCell ref="B111:B113"/>
-    <mergeCell ref="A110:A113"/>
-    <mergeCell ref="E124:E126"/>
-    <mergeCell ref="E100:E101"/>
-    <mergeCell ref="E102:E103"/>
-    <mergeCell ref="E104:E105"/>
-    <mergeCell ref="E106:E107"/>
-    <mergeCell ref="E108:E109"/>
-    <mergeCell ref="E111:E113"/>
-    <mergeCell ref="A123:A126"/>
-    <mergeCell ref="A106:A107"/>
-    <mergeCell ref="A108:A109"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="E72:E73"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="A72:A74"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="A56:A59"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="A63:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="A69:A71"/>
-    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="A37:A43"/>
+    <mergeCell ref="A2:A36"/>
+    <mergeCell ref="B14:B36"/>
+    <mergeCell ref="A94:A96"/>
+    <mergeCell ref="B97:B98"/>
+    <mergeCell ref="A97:A99"/>
+    <mergeCell ref="A100:A101"/>
+    <mergeCell ref="A102:A103"/>
     <mergeCell ref="E75:E77"/>
     <mergeCell ref="E79:E81"/>
     <mergeCell ref="E82:E83"/>
@@ -8580,24 +8409,56 @@
     <mergeCell ref="B79:B81"/>
     <mergeCell ref="A79:A83"/>
     <mergeCell ref="E120:E122"/>
-    <mergeCell ref="A94:A96"/>
-    <mergeCell ref="B97:B98"/>
-    <mergeCell ref="A97:A99"/>
-    <mergeCell ref="A100:A101"/>
-    <mergeCell ref="A102:A103"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="A37:A43"/>
-    <mergeCell ref="A2:A36"/>
-    <mergeCell ref="B14:B36"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="A44:A48"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="A49:A52"/>
-    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="E72:E73"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="A72:A74"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="A56:A59"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="A63:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="B111:B113"/>
+    <mergeCell ref="A110:A113"/>
+    <mergeCell ref="E124:E126"/>
+    <mergeCell ref="E100:E101"/>
+    <mergeCell ref="E102:E103"/>
+    <mergeCell ref="E104:E105"/>
+    <mergeCell ref="E106:E107"/>
+    <mergeCell ref="E108:E109"/>
+    <mergeCell ref="E111:E113"/>
+    <mergeCell ref="A123:A126"/>
+    <mergeCell ref="A106:A107"/>
+    <mergeCell ref="A108:A109"/>
+    <mergeCell ref="F117:F118"/>
+    <mergeCell ref="E115:E118"/>
+    <mergeCell ref="E84:E86"/>
+    <mergeCell ref="E88:E89"/>
+    <mergeCell ref="E91:E92"/>
+    <mergeCell ref="E95:E96"/>
+    <mergeCell ref="A143:A146"/>
+    <mergeCell ref="B143:B146"/>
+    <mergeCell ref="A129:A131"/>
+    <mergeCell ref="B130:B131"/>
+    <mergeCell ref="C117:C118"/>
+    <mergeCell ref="A114:A118"/>
+    <mergeCell ref="A132:A133"/>
+    <mergeCell ref="A147:A148"/>
+    <mergeCell ref="B147:B148"/>
+    <mergeCell ref="A149:A150"/>
+    <mergeCell ref="B149:B150"/>
+    <mergeCell ref="A151:A152"/>
+    <mergeCell ref="B151:B152"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>